<commit_message>
Unit 2301 and 2302 fixes II
</commit_message>
<xml_diff>
--- a/book2/2302/file/2302-05.xlsx
+++ b/book2/2302/file/2302-05.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\rin2-dev\2302\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\rin2\book2\2302\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="5" r:id="rId1"/>
     <sheet name="List2" sheetId="6" r:id="rId2"/>
     <sheet name="List3" sheetId="7" r:id="rId3"/>
     <sheet name="List4" sheetId="1" r:id="rId4"/>
+    <sheet name="List5" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="15">
   <si>
     <t>jan</t>
   </si>
@@ -271,7 +272,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -392,7 +392,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2052,6 +2051,521 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="sl-SI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sl-SI"/>
+              <a:t>Prodaja pic</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sl-SI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List5!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mesna</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>List5!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>maj</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>avg</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>okt</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>List5!$B$2:$M$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F064-42B6-907E-2A9B99999F72}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List5!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>brezmesna</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>List5!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>maj</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>avg</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>okt</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>List5!$B$3:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F064-42B6-907E-2A9B99999F72}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="50"/>
+        <c:overlap val="100"/>
+        <c:axId val="466347056"/>
+        <c:axId val="466346400"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="466347056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sl-SI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="466346400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="466346400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="500"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sl-SI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="466347056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="100"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sl-SI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sl-SI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2212,6 +2726,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -3770,6 +4324,525 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4458,6 +5531,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafikon 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Officeova tema">
   <a:themeElements>
@@ -4723,7 +5839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5336,4 +6452,158 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="13" width="5.33203125" customWidth="1"/>
+    <col min="14" max="15" width="7.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="6"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4">
+        <v>197</v>
+      </c>
+      <c r="C2" s="5">
+        <v>192</v>
+      </c>
+      <c r="D2" s="5">
+        <v>206</v>
+      </c>
+      <c r="E2" s="5">
+        <v>196</v>
+      </c>
+      <c r="F2" s="5">
+        <v>188</v>
+      </c>
+      <c r="G2" s="5">
+        <v>207</v>
+      </c>
+      <c r="H2" s="5">
+        <v>241</v>
+      </c>
+      <c r="I2" s="5">
+        <v>237</v>
+      </c>
+      <c r="J2" s="5">
+        <v>226</v>
+      </c>
+      <c r="K2" s="5">
+        <v>218</v>
+      </c>
+      <c r="L2" s="5">
+        <v>214</v>
+      </c>
+      <c r="M2" s="5">
+        <v>201</v>
+      </c>
+      <c r="N2" s="9">
+        <f>SUM(B2:M2)</f>
+        <v>2523</v>
+      </c>
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5">
+        <v>56</v>
+      </c>
+      <c r="D3" s="5">
+        <v>68</v>
+      </c>
+      <c r="E3" s="5">
+        <v>78</v>
+      </c>
+      <c r="F3" s="5">
+        <v>89</v>
+      </c>
+      <c r="G3" s="5">
+        <v>117</v>
+      </c>
+      <c r="H3" s="5">
+        <v>128</v>
+      </c>
+      <c r="I3" s="5">
+        <v>125</v>
+      </c>
+      <c r="J3" s="5">
+        <v>105</v>
+      </c>
+      <c r="K3" s="5">
+        <v>63</v>
+      </c>
+      <c r="L3" s="5">
+        <v>58</v>
+      </c>
+      <c r="M3" s="5">
+        <v>49</v>
+      </c>
+      <c r="N3" s="9">
+        <f>SUM(B3:M3)</f>
+        <v>983</v>
+      </c>
+      <c r="O3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>